<commit_message>
plotted heatmap exo peps
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/CC-GO-summary.xlsx
+++ b/analyses/unipept/GO-terms/CC-GO-summary.xlsx
@@ -18,6 +18,7 @@
     <sheet name="332-undigested" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="PCA-input-DIATOM" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="PCA-input-BACTERIA" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="venn-input" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="198">
   <si>
     <t xml:space="preserve">DIATOM</t>
   </si>
@@ -502,9 +503,6 @@
     <t xml:space="preserve">particle</t>
   </si>
   <si>
-    <t xml:space="preserve">Membrane:cytosol</t>
-  </si>
-  <si>
     <t xml:space="preserve">cumulative</t>
   </si>
   <si>
@@ -523,12 +521,21 @@
     <t xml:space="preserve">T12-325</t>
   </si>
   <si>
+    <t xml:space="preserve">T0-329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2-330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T5-331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T12-332</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009538 photosystem I reaction center</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009535 chloroplast thylakoid membrane</t>
   </si>
   <si>
@@ -577,40 +584,46 @@
     <t xml:space="preserve">GO:0009522 photosystem I</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0030126 coatomer vesicle coat</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0015935 small ribosomal subunit</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0005788 endoplasmic reticulum lumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009523 photosystem II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009539 photosystem II reaction center </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000139 Golgi membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005741 mitochondrial outer membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005750 mitochondrial respiratory chain complex III </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005762 mitochondrial large ribosomal subunit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009534 chloroplast thylakoid</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0030126 COPI vesicle coat</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005788 endoplasmic reticulum lumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009523 photosystem II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009539 photosystem II reaction center </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0000139 Golgi membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005741 mitochondrial outer membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005750 mitochondrial respiratory chain complex III </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005762 mitochondrial large ribosomal subunit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009534 chloroplast thylakoid</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0031361 integral component of thylakoid membrane</t>
   </si>
   <si>
     <t xml:space="preserve">Membrane:cytoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venn</t>
   </si>
 </sst>
 </file>
@@ -625,6 +638,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -744,7 +758,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -790,10 +804,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -876,13 +886,13 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,10 +1653,10 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.21"/>
   </cols>
@@ -1656,7 +1666,7 @@
         <v>64</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,31 +1674,31 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,12 +1887,12 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,57 +1902,57 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J22" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J24" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J25" s="0" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,10 +1963,74 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1972,11 +2046,11 @@
       <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.35"/>
@@ -2860,7 +2934,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2879,7 +2953,7 @@
       <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.88"/>
   </cols>
@@ -3410,7 +3484,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3429,7 +3503,7 @@
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
@@ -3923,7 +3997,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3939,10 +4013,10 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4326,7 +4400,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -4339,13 +4413,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4378,6 +4452,10 @@
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">A4+A5</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -4446,6 +4524,10 @@
       <c r="F8" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">A8+A10+A12</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -5154,7 +5236,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5173,7 +5255,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5357,7 +5439,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5373,10 +5455,10 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5585,7 +5667,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5598,25 +5680,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:AA52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA18" activeCellId="0" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="55.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="26.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="0" t="s">
-        <v>157</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -5634,50 +5713,62 @@
       <c r="E2" s="0" t="n">
         <v>325</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>332</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="S2" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>163</v>
+      <c r="Y2" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,58 +5787,55 @@
       <c r="E3" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <f aca="false">SUM(B3:E3)</f>
         <v>92</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="N3" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="0" t="n">
+      <c r="O3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="O3" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <f aca="false">J6+J14+J18+J19</f>
+      <c r="S3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">N6+N14+N18+N19</f>
         <v>8</v>
       </c>
-      <c r="Q3" s="0" t="n">
-        <f aca="false">K6+K14+K18+K19</f>
-        <v>2</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <f aca="false">L6+L14+L18+L19</f>
+      <c r="U3" s="0" t="n">
+        <f aca="false">O6+O14+O18+O19</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <f aca="false">P6+P14+P18+P19</f>
         <v>8</v>
       </c>
-      <c r="S3" s="0" t="n">
-        <f aca="false">M6+M14+M18+M19</f>
+      <c r="W3" s="0" t="n">
+        <f aca="false">Q6+Q14+Q18+Q19</f>
         <v>7</v>
       </c>
-      <c r="T3" s="0" t="n">
-        <f aca="false">P5/P17</f>
-        <v>10.25</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <f aca="false">Q5/Q17</f>
-        <v>0.176470588235294</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <f aca="false">R5/R17</f>
-        <v>14</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>165</v>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5766,43 +5854,55 @@
       <c r="E4" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <f aca="false">SUM(B4:E4)</f>
         <v>76</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="M4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="n">
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="Q4" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <f aca="false">J4+J5+J29+J32</f>
+      <c r="S4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <f aca="false">N4+N5+N29+N32</f>
         <v>46</v>
       </c>
-      <c r="Q4" s="0" t="n">
-        <f aca="false">K4+K5+K29+K32</f>
-        <v>2</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <f aca="false">L4+L5+L29+L32</f>
+      <c r="U4" s="0" t="n">
+        <f aca="false">O4+O5+O29+O32</f>
+        <v>2</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <f aca="false">P4+P5+P29+P32</f>
         <v>34</v>
       </c>
-      <c r="S4" s="0" t="n">
-        <f aca="false">M4+M5+M29+M32</f>
+      <c r="W4" s="0" t="n">
+        <f aca="false">Q4+Q5+Q29+Q32</f>
         <v>30</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5821,43 +5921,55 @@
       <c r="E5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <f aca="false">SUM(B5:E5)</f>
         <v>34</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="M5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="N5" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="K5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="0" t="n">
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="Q5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="0" t="n">
-        <f aca="false">J3+J15</f>
+      <c r="T5" s="0" t="n">
+        <f aca="false">N3+N15</f>
         <v>41</v>
       </c>
-      <c r="Q5" s="0" t="n">
-        <f aca="false">K3+K15</f>
+      <c r="U5" s="0" t="n">
+        <f aca="false">O3+O15</f>
         <v>3</v>
       </c>
-      <c r="R5" s="0" t="n">
-        <f aca="false">L3+L15</f>
+      <c r="V5" s="0" t="n">
+        <f aca="false">P3+P15</f>
         <v>28</v>
       </c>
-      <c r="S5" s="0" t="n">
-        <f aca="false">M3+M15</f>
+      <c r="W5" s="0" t="n">
+        <f aca="false">Q3+Q15</f>
         <v>24</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5876,39 +5988,51 @@
       <c r="E6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <f aca="false">SUM(B6:E6)</f>
         <v>17</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="M6" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="0" t="n">
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="Q6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O6" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="P6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>1</v>
+      <c r="S6" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5924,38 +6048,50 @@
       <c r="D7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <f aca="false">SUM(B7:E7)</f>
         <v>14</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="N7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="L7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="P7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5966,42 +6102,54 @@
       <c r="C8" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <f aca="false">SUM(B8:E8)</f>
         <v>13</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="0" t="n">
+      <c r="M8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="P8" s="0" t="n">
-        <f aca="false">J34+J9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <f aca="false">K34+K9</f>
-        <v>2</v>
-      </c>
-      <c r="R8" s="0" t="n">
-        <f aca="false">L34+L9</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <f aca="false">N34+N9</f>
+        <v>2</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <f aca="false">O34+O9</f>
+        <v>2</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <f aca="false">P34+P9</f>
         <v>3</v>
       </c>
-      <c r="S8" s="0" t="n">
-        <f aca="false">M34+M9</f>
+      <c r="W8" s="0" t="n">
+        <f aca="false">Q34+Q9</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6018,42 +6166,54 @@
       <c r="D9" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <f aca="false">SUM(B9:E9)</f>
         <v>6</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L9" s="0" t="n">
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <f aca="false">J33+J8</f>
-        <v>1</v>
-      </c>
       <c r="Q9" s="0" t="n">
-        <f aca="false">K33+K8</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <f aca="false">N33+N8</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <f aca="false">O33+O8</f>
         <v>13</v>
       </c>
-      <c r="R9" s="0" t="n">
-        <f aca="false">L33+L8</f>
-        <v>0</v>
-      </c>
-      <c r="S9" s="0" t="n">
-        <f aca="false">M33+M8</f>
+      <c r="V9" s="0" t="n">
+        <f aca="false">P33+P8</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <f aca="false">Q33+Q8</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6064,42 +6224,54 @@
       <c r="C10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <f aca="false">SUM(B10:E10)</f>
         <v>5</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="M10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="P10" s="0" t="n">
-        <f aca="false">J20+J27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <f aca="false">K20+K27</f>
-        <v>0</v>
-      </c>
-      <c r="R10" s="0" t="n">
-        <f aca="false">L20+L27</f>
-        <v>0</v>
-      </c>
-      <c r="S10" s="0" t="n">
-        <f aca="false">M20+M27</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <f aca="false">N20+N27</f>
+        <v>2</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <f aca="false">O20+O27</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <f aca="false">P20+P27</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <f aca="false">Q20+Q27</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6113,38 +6285,50 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <f aca="false">SUM(B11:E11)</f>
         <v>5</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J11" s="0" t="n">
+      <c r="M11" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="N11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>176</v>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" s="0" t="n">
+      <c r="S11" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6158,42 +6342,54 @@
       <c r="C12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <f aca="false">SUM(B12:E12)</f>
         <v>4</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>178</v>
+      <c r="M12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="P12" s="0" t="n">
-        <f aca="false">J17+J25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <f aca="false">K17+K25</f>
-        <v>2</v>
-      </c>
-      <c r="R12" s="0" t="n">
-        <f aca="false">L17+L25</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="0" t="n">
-        <f aca="false">M17+M25</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <f aca="false">N17+N25</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <f aca="false">O17+O25</f>
+        <v>2</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <f aca="false">P17+P25</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <f aca="false">Q17+Q25</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6207,42 +6403,54 @@
       <c r="C13" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <f aca="false">SUM(B13:E13)</f>
         <v>4</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="0" t="n">
+      <c r="M13" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="P13" s="0" t="n">
-        <f aca="false">J21+J22+J23+J24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <f aca="false">K21+K22+K23+K24</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <f aca="false">N21+N22+N23+N24</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <f aca="false">O21+O22+O23+O24</f>
         <v>3</v>
       </c>
-      <c r="R13" s="0" t="n">
-        <f aca="false">L21+L22+L23+L24</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="0" t="n">
-        <f aca="false">M21+M22+M23+M24</f>
+      <c r="V13" s="0" t="n">
+        <f aca="false">P21+P22+P23+P24</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <f aca="false">Q21+Q22+Q23+Q24</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6259,38 +6467,50 @@
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="J14" s="0" t="n">
         <f aca="false">SUM(B14:E14)</f>
         <v>4</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>179</v>
+      <c r="M14" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="R14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6304,42 +6524,50 @@
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="J15" s="0" t="n">
         <f aca="false">SUM(B15:E15)</f>
         <v>4</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>182</v>
+      <c r="N15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="P15" s="0" t="n">
-        <f aca="false">J16+J11</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <f aca="false">K16+K11</f>
-        <v>2</v>
-      </c>
-      <c r="R15" s="0" t="n">
-        <f aca="false">L16+L11</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="0" t="n">
-        <f aca="false">M16+M11</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6353,38 +6581,54 @@
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="J16" s="0" t="n">
         <f aca="false">SUM(B16:E16)</f>
         <v>3</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>183</v>
+      <c r="M16" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="0" t="n">
+      <c r="S16" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <f aca="false">N16+N11</f>
+        <v>6</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <f aca="false">O16+O11</f>
+        <v>2</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <f aca="false">P16+P11</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <f aca="false">Q16+Q11</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6395,42 +6639,54 @@
       <c r="C17" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <f aca="false">SUM(B17:E17)</f>
         <v>2</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="3" t="s">
+      <c r="M17" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P17" s="0" t="n">
-        <f aca="false">J10+J12+J7</f>
+      <c r="T17" s="0" t="n">
+        <f aca="false">N10+N12+N7</f>
         <v>4</v>
       </c>
-      <c r="Q17" s="0" t="n">
-        <f aca="false">K10+K12+K7</f>
+      <c r="U17" s="0" t="n">
+        <f aca="false">O10+O12+O7</f>
         <v>17</v>
       </c>
-      <c r="R17" s="0" t="n">
-        <f aca="false">L10+L12+L7</f>
-        <v>2</v>
-      </c>
-      <c r="S17" s="0" t="n">
-        <f aca="false">M10+M12+M7</f>
+      <c r="V17" s="0" t="n">
+        <f aca="false">P10+P12+P7</f>
+        <v>2</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <f aca="false">Q10+Q12+Q7</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6444,23 +6700,23 @@
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <f aca="false">SUM(B18:E18)</f>
         <v>2</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6474,23 +6730,23 @@
       <c r="E19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <f aca="false">SUM(B19:E19)</f>
         <v>2</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6501,23 +6757,23 @@
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <f aca="false">SUM(B20:E20)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6528,23 +6784,23 @@
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <f aca="false">SUM(B21:E21)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6555,23 +6811,23 @@
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <f aca="false">SUM(B22:E22)</f>
         <v>1</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6582,23 +6838,23 @@
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <f aca="false">SUM(B23:E23)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6609,23 +6865,23 @@
       <c r="C24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <f aca="false">SUM(B24:E24)</f>
         <v>1</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6636,23 +6892,23 @@
       <c r="B25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <f aca="false">SUM(B25:E25)</f>
         <v>1</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6663,23 +6919,23 @@
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <f aca="false">SUM(B26:E26)</f>
         <v>1</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6690,23 +6946,23 @@
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="J27" s="0" t="n">
         <f aca="false">SUM(B27:E27)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6717,23 +6973,23 @@
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="J28" s="0" t="n">
         <f aca="false">SUM(B28:E28)</f>
         <v>1</v>
       </c>
-      <c r="I28" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6744,23 +7000,23 @@
       <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="J29" s="0" t="n">
         <f aca="false">SUM(B29:E29)</f>
         <v>1</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="0" t="n">
+      <c r="M29" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6771,23 +7027,23 @@
       <c r="E30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="J30" s="0" t="n">
         <f aca="false">SUM(B30:E30)</f>
         <v>1</v>
       </c>
-      <c r="I30" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="0" t="n">
+      <c r="M30" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6798,23 +7054,23 @@
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="J31" s="0" t="n">
         <f aca="false">SUM(B31:E31)</f>
         <v>1</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="0" t="n">
+      <c r="M31" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6825,23 +7081,23 @@
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="J32" s="0" t="n">
         <f aca="false">SUM(B32:E32)</f>
         <v>1</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" s="0" t="n">
+      <c r="M32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6852,23 +7108,23 @@
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="J33" s="0" t="n">
         <f aca="false">SUM(B33:E33)</f>
         <v>1</v>
       </c>
-      <c r="I33" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" s="0" t="n">
+      <c r="M33" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6879,23 +7135,23 @@
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="J34" s="0" t="n">
         <f aca="false">SUM(B34:E34)</f>
         <v>1</v>
       </c>
-      <c r="I34" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" s="0" t="n">
+      <c r="M34" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6918,7 +7174,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>